<commit_message>
mss19r gotowy pus poprawki
</commit_message>
<xml_diff>
--- a/Statystyki_2018/Template/wab.xlsx
+++ b/Statystyki_2018/Template/wab.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev-Klon-wap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myProjects\prv\statystyki\Statystyki_2018\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{97F8F23C-A234-4DBA-9391-938080178380}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637433BB-7EDD-418F-B638-775854F85E20}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="206"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="206" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="51">
   <si>
     <t>Sąd / Wydział</t>
   </si>
@@ -57,13 +58,153 @@
   <si>
     <t xml:space="preserve">% powyżej 30
 dni do razem </t>
+  </si>
+  <si>
+    <t>Liczba złożonych wniosków o przyznanie wynagrodzenia biegłemu (tłumaczowi)</t>
+  </si>
+  <si>
+    <t>Liczba rozpoznanych wniosków o przyznanie wynagrodzenia biegłemu (tłumaczowi), licząc od daty wpływu wniosku</t>
+  </si>
+  <si>
+    <t>Liczba wniosków przekazanych do oddziału finansowego, licząc od daty uprawomocnienia orzeczenia</t>
+  </si>
+  <si>
+    <t>Liczba wniosków, w których wypłacono wynagrodzenie biegłemu (tłumaczowi), licząc od daty przekazania dokumentacji do oddziału finansowego</t>
+  </si>
+  <si>
+    <t>w tym w terminie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">do 7 dni </t>
+  </si>
+  <si>
+    <t>od 7 do 30 dni</t>
+  </si>
+  <si>
+    <t>powyżej 30 dni lub nie wypłacone</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Informacja dot. pracy biegłych sądowych (WAB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="238"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Wysłano</t>
+  </si>
+  <si>
+    <t>Zwrócono z opinią</t>
+  </si>
+  <si>
+    <t>Zwrócono bez opinii</t>
+  </si>
+  <si>
+    <t>Zwrócono po terminie</t>
+  </si>
+  <si>
+    <t>Termin do sporządzenia przedłużono</t>
+  </si>
+  <si>
+    <t>Ponaglono o wykonanie opinii</t>
+  </si>
+  <si>
+    <t>W terminie 14 dni wydano post. o wynagrodzeniu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skierowano do wykonania w terminie 14 dni </t>
+  </si>
+  <si>
+    <t>Sąd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ilość złożonych opinii , tłumaczeń </t>
+  </si>
+  <si>
+    <t>Rozpoznane wnioski o przyznanie wynagrodzenia biegłemu (tłumaczowi), licząc od daty wpływu wniosku</t>
+  </si>
+  <si>
+    <t>ilość przypadków przekazania księgowości polecenia wypłaty wynagrodzenia biegłemu</t>
+  </si>
+  <si>
+    <t>razem</t>
+  </si>
+  <si>
+    <t>w tym w terminie</t>
+  </si>
+  <si>
+    <t>do 14 dni</t>
+  </si>
+  <si>
+    <t>pow.14 do 30 dni</t>
+  </si>
+  <si>
+    <t>powyżej 30 dni do 3 m-cy</t>
+  </si>
+  <si>
+    <t>powyżej 3 m-cy do 6 m-cy</t>
+  </si>
+  <si>
+    <t>powyżej 6 m-cy</t>
+  </si>
+  <si>
+    <t>Sądy Rejonowe</t>
+  </si>
+  <si>
+    <t>poprzedni rok</t>
+  </si>
+  <si>
+    <t>obecny rok</t>
+  </si>
+  <si>
+    <t>RAZEM</t>
+  </si>
+  <si>
+    <t>tab. 2</t>
+  </si>
+  <si>
+    <t>ilość niezrealizowanych wypłat wynagrodzeń wg stanu na 31 marca 2019 r. za okres 1 stycznia 2015 – do końca okresu</t>
+  </si>
+  <si>
+    <t>* przypadki 3 najstarszych niezrealizowanych wypłat, licząc od dnia złożenia opinii przez biegłego</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>Sąd Rejonowy</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tab.1 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -76,16 +217,65 @@
       <family val="1"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -108,19 +298,110 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,102 +800,102 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
     </row>
     <row r="2" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
     </row>
     <row r="3" spans="2:13" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="2" t="s">
+      <c r="I3" s="3"/>
+      <c r="J3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -638,14 +919,134 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B1:O4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:O4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+    </row>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="2:15" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+    </row>
+  </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <mergeCells count="11">
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:L3"/>
+  </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0">
@@ -656,14 +1057,64 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B1:I2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:I2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="6" max="6" width="12.77734375" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="2:9" ht="58.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="B1:I1"/>
+  </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0">
@@ -671,4 +1122,249 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12Strona &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F186EE30-C4E1-426B-BAD0-8479A0B7F916}">
+  <dimension ref="A1:T13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+    </row>
+    <row r="3" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="8"/>
+    </row>
+    <row r="4" spans="1:20" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="O4" s="8"/>
+    </row>
+    <row r="5" spans="1:20" ht="20.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="12"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="17"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="19"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="76.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="23"/>
+    </row>
+    <row r="12" spans="1:20" ht="20.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="23"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="O2:T2"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="O3:O4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>